<commit_message>
this file updates the readme from excel file
</commit_message>
<xml_diff>
--- a/DataWorks Progress Plan.xlsx
+++ b/DataWorks Progress Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ebde79330a9dc7c/DataWorks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{E66B0224-F8D0-764B-9225-0937AE3AA255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8327B834-5386-2E4E-8ED3-BAE313CF5804}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{E66B0224-F8D0-764B-9225-0937AE3AA255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60FB334F-C7BB-C648-9C88-DE988EDDE67F}"/>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="2460" windowWidth="27640" windowHeight="16660" xr2:uid="{23DF04E5-15B2-E549-A06F-1367FF6B7B05}"/>
+    <workbookView xWindow="1760" yWindow="760" windowWidth="27640" windowHeight="16660" xr2:uid="{23DF04E5-15B2-E549-A06F-1367FF6B7B05}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 - October" sheetId="1" r:id="rId1"/>
@@ -38,10 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
-  <si>
-    <t>Resources</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Week</t>
   </si>
@@ -61,13 +58,28 @@
     <t>Job Search</t>
   </si>
   <si>
-    <t>Career Progress Plan</t>
-  </si>
-  <si>
     <t>W3 Schools - SQL</t>
   </si>
   <si>
     <t>basics, joins, operators</t>
+  </si>
+  <si>
+    <t>SQL Resources</t>
+  </si>
+  <si>
+    <t>Big Data Resources</t>
+  </si>
+  <si>
+    <t>DS Resources</t>
+  </si>
+  <si>
+    <t>Job Search Resources</t>
+  </si>
+  <si>
+    <t>Working on PySpark project</t>
+  </si>
+  <si>
+    <t>Kaggle Brzilian olist</t>
   </si>
 </sst>
 </file>
@@ -120,11 +132,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -153,6 +162,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -472,96 +485,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9341BC7-A261-014D-88E7-187B049BB749}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.83203125" style="4"/>
-    <col min="3" max="16384" width="15.83203125" style="3"/>
+    <col min="1" max="16384" width="16.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="46" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" s="4" customFormat="1" ht="23" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>8</v>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:J2"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" xr:uid="{658B331E-9B00-0144-BE2E-36F30C322064}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{CEEF0E53-0E29-3146-951B-BC31E806EBA7}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{0B65A4FE-628B-6346-B2D4-900491C384AE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add this new activity to the file
</commit_message>
<xml_diff>
--- a/DataWorks Progress Plan.xlsx
+++ b/DataWorks Progress Plan.xlsx
@@ -8,14 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ebde79330a9dc7c/DataWorks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{E66B0224-F8D0-764B-9225-0937AE3AA255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{610E7A3F-83DE-4D6F-8826-196DD5142D9B}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="8_{E66B0224-F8D0-764B-9225-0937AE3AA255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7CC9253-A56C-449A-9DCB-C188A63D41A8}"/>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="760" windowWidth="27640" windowHeight="16660" activeTab="2" xr2:uid="{23DF04E5-15B2-E549-A06F-1367FF6B7B05}"/>
+    <workbookView xWindow="1760" yWindow="760" windowWidth="27640" windowHeight="16660" xr2:uid="{23DF04E5-15B2-E549-A06F-1367FF6B7B05}"/>
   </bookViews>
   <sheets>
-    <sheet name="2025 - October" sheetId="1" r:id="rId1"/>
-    <sheet name="2025 - November" sheetId="4" r:id="rId2"/>
-    <sheet name="2025 - December" sheetId="5" r:id="rId3"/>
+    <sheet name="2026 - January" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -486,7 +484,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9341BC7-A261-014D-88E7-187B049BB749}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -547,138 +547,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{963248B5-344B-4333-9A21-2912F38840C6}">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="16.125" defaultRowHeight="15.75" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="16.125" style="6"/>
-    <col min="2" max="16384" width="16.125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="39.75">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="30.75">
-      <c r="A2" s="6">
-        <v>46023</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{29A3F8FD-D284-4567-A4DD-A5E44DC8FCB8}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{1326FFCB-3BB2-4AD6-9F78-B6BDAFBBF44C}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{152B27F7-027B-4E3B-9012-7C6679E06D18}">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="16.125" defaultRowHeight="15.75" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="16.125" style="6"/>
-    <col min="2" max="16384" width="16.125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="39.75">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="30.75">
-      <c r="A2" s="6">
-        <v>46023</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{BC9884AF-35C3-43D3-8CC9-29DF859F9B08}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{41CB3F3A-3633-4980-9C58-074ED3ED8B05}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>